<commit_message>
analise de dados adicionado
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,32 +470,15 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Julia</t>
+          <t>Brendon</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>$2b$12$ix/RJ1kyAGpk.K4HZX7f.un4aShA4Gtp08cDo.mTbSXml0UnvUPei</t>
+          <t>$2b$12$.BvYnlk164DiJ9jTsNHK7OAkq045fG9Ma6Vk/mWfS6pBozLIyjlMS</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
-        <is>
-          <t>funcionario</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Brendon</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>$2b$12$.BvYnlk164DiJ9jTsNHK7OAkq045fG9Ma6Vk/mWfS6pBozLIyjlMS</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
         <is>
           <t>admin</t>
         </is>

</xml_diff>

<commit_message>
Adicionado filtro de dados
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,23 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Charles</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>$2b$12$QQjbf5ap2t8m6gHqIJ5WxeUHn4VJFcDblqQShQWC92oupeMbk61S.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>funcionario</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>